<commit_message>
Fixed Bugs & Updates entered info in message
</commit_message>
<xml_diff>
--- a/Attendata.xlsx
+++ b/Attendata.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bhuvansa/Desktop/Projects/unsorted/Whatsappbot/FourthSem/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bhuvansa/Desktop/Projects/unsorted/Whatsappbot/WhatsappMarksBot/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{401CCC4E-C22A-0846-8B91-38EA77651930}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F73C5C9B-0EF3-B348-A6B0-62C474482CA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-33600" yWindow="15580" windowWidth="33600" windowHeight="21000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-33600" yWindow="0" windowWidth="33600" windowHeight="21000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CIE (2)" sheetId="2" r:id="rId1"/>
@@ -558,7 +558,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -679,11 +679,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFill="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
@@ -731,13 +742,13 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyProtection="1"/>
@@ -750,23 +761,18 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -874,9 +880,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -914,7 +920,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1020,7 +1026,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1162,7 +1168,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1173,7 +1179,7 @@
   <dimension ref="A1:J32"/>
   <sheetViews>
     <sheetView showRuler="0" zoomScale="103" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11:A27"/>
+      <selection activeCell="H30" sqref="H30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1845,7 +1851,7 @@
   <dimension ref="A1:S78"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="P9" sqref="P9:Q9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1900,7 +1906,7 @@
       <c r="N3" s="13">
         <v>9901043233</v>
       </c>
-      <c r="O3" s="26"/>
+      <c r="O3" s="12"/>
     </row>
     <row r="4" spans="1:19" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="20" t="s">
@@ -1948,34 +1954,34 @@
       <c r="C9" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D9" s="17" t="s">
+      <c r="D9" s="26" t="s">
         <v>158</v>
       </c>
-      <c r="E9" s="17"/>
-      <c r="F9" s="29" t="s">
+      <c r="E9" s="27"/>
+      <c r="F9" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="G9" s="30"/>
-      <c r="H9" s="27" t="s">
+      <c r="G9" s="25"/>
+      <c r="H9" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="I9" s="28"/>
-      <c r="J9" s="29" t="s">
+      <c r="I9" s="25"/>
+      <c r="J9" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="K9" s="30"/>
-      <c r="L9" s="29" t="s">
+      <c r="K9" s="25"/>
+      <c r="L9" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="M9" s="30"/>
-      <c r="N9" s="29" t="s">
+      <c r="M9" s="25"/>
+      <c r="N9" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="O9" s="30"/>
-      <c r="P9" s="29" t="s">
+      <c r="O9" s="25"/>
+      <c r="P9" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="Q9" s="30"/>
+      <c r="Q9" s="25"/>
       <c r="R9" s="23" t="s">
         <v>14</v>
       </c>
@@ -1987,46 +1993,46 @@
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="3"/>
-      <c r="D10" s="18" t="s">
+      <c r="D10" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="E10" s="24" t="s">
+      <c r="E10" s="7" t="s">
         <v>160</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G10" s="24" t="s">
+      <c r="G10" s="7" t="s">
         <v>159</v>
       </c>
       <c r="H10" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="I10" s="24" t="s">
+      <c r="I10" s="7" t="s">
         <v>159</v>
       </c>
       <c r="J10" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="K10" s="24" t="s">
+      <c r="K10" s="7" t="s">
         <v>159</v>
       </c>
       <c r="L10" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="M10" s="24" t="s">
+      <c r="M10" s="7" t="s">
         <v>159</v>
       </c>
       <c r="N10" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="O10" s="24" t="s">
+      <c r="O10" s="7" t="s">
         <v>159</v>
       </c>
       <c r="P10" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="Q10" s="24" t="s">
+      <c r="Q10" s="7" t="s">
         <v>159</v>
       </c>
       <c r="R10" s="1"/>
@@ -2041,46 +2047,46 @@
       <c r="C11" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="D11" s="19" t="s">
+      <c r="D11" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="E11" s="19">
+      <c r="E11" s="18">
         <v>99</v>
       </c>
       <c r="F11" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="G11" s="25">
+      <c r="G11" s="19">
         <v>99</v>
       </c>
       <c r="H11" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="I11" s="25">
+      <c r="I11" s="19">
         <v>99</v>
       </c>
       <c r="J11" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="K11" s="25">
+      <c r="K11" s="19">
         <v>99</v>
       </c>
       <c r="L11" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="M11" s="25">
+      <c r="M11" s="19">
         <v>99</v>
       </c>
       <c r="N11" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="O11" s="25">
+      <c r="O11" s="19">
         <v>99</v>
       </c>
       <c r="P11" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="Q11" s="25">
+      <c r="Q11" s="19">
         <v>99</v>
       </c>
       <c r="R11" s="1"/>
@@ -2107,37 +2113,37 @@
       <c r="F12" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="G12" s="25">
+      <c r="G12" s="19">
         <v>99</v>
       </c>
       <c r="H12" s="2">
         <v>23</v>
       </c>
-      <c r="I12" s="25">
+      <c r="I12" s="19">
         <v>99</v>
       </c>
       <c r="J12" s="2">
         <v>22</v>
       </c>
-      <c r="K12" s="25">
+      <c r="K12" s="19">
         <v>99</v>
       </c>
       <c r="L12" s="2">
         <v>30</v>
       </c>
-      <c r="M12" s="25">
+      <c r="M12" s="19">
         <v>99</v>
       </c>
       <c r="N12" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="O12" s="25">
+      <c r="O12" s="19">
         <v>99</v>
       </c>
       <c r="P12" s="2">
         <v>40</v>
       </c>
-      <c r="Q12" s="25">
+      <c r="Q12" s="19">
         <v>99</v>
       </c>
       <c r="R12" s="1"/>
@@ -2164,37 +2170,37 @@
       <c r="F13" s="2">
         <v>27</v>
       </c>
-      <c r="G13" s="25">
+      <c r="G13" s="19">
         <v>99</v>
       </c>
       <c r="H13" s="2">
         <v>29</v>
       </c>
-      <c r="I13" s="25">
+      <c r="I13" s="19">
         <v>99</v>
       </c>
       <c r="J13" s="2">
         <v>29</v>
       </c>
-      <c r="K13" s="25">
+      <c r="K13" s="19">
         <v>99</v>
       </c>
       <c r="L13" s="2">
         <v>33</v>
       </c>
-      <c r="M13" s="25">
+      <c r="M13" s="19">
         <v>99</v>
       </c>
       <c r="N13" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="O13" s="25">
+      <c r="O13" s="19">
         <v>99</v>
       </c>
       <c r="P13" s="2">
         <v>38</v>
       </c>
-      <c r="Q13" s="25">
+      <c r="Q13" s="19">
         <v>99</v>
       </c>
       <c r="R13" s="1"/>
@@ -2221,37 +2227,37 @@
       <c r="F14" s="2">
         <v>15</v>
       </c>
-      <c r="G14" s="25">
+      <c r="G14" s="19">
         <v>99</v>
       </c>
       <c r="H14" s="2">
         <v>9</v>
       </c>
-      <c r="I14" s="25">
+      <c r="I14" s="19">
         <v>99</v>
       </c>
       <c r="J14" s="2">
         <v>12</v>
       </c>
-      <c r="K14" s="25">
+      <c r="K14" s="19">
         <v>99</v>
       </c>
       <c r="L14" s="2">
         <v>14</v>
       </c>
-      <c r="M14" s="25">
+      <c r="M14" s="19">
         <v>99</v>
       </c>
       <c r="N14" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="O14" s="25">
+      <c r="O14" s="19">
         <v>99</v>
       </c>
       <c r="P14" s="2">
         <v>19</v>
       </c>
-      <c r="Q14" s="25">
+      <c r="Q14" s="19">
         <v>99</v>
       </c>
       <c r="R14" s="1"/>
@@ -2278,37 +2284,37 @@
       <c r="F15" s="2">
         <v>28</v>
       </c>
-      <c r="G15" s="25">
+      <c r="G15" s="19">
         <v>99</v>
       </c>
       <c r="H15" s="2">
         <v>27</v>
       </c>
-      <c r="I15" s="25">
+      <c r="I15" s="19">
         <v>99</v>
       </c>
       <c r="J15" s="2">
         <v>33</v>
       </c>
-      <c r="K15" s="25">
+      <c r="K15" s="19">
         <v>99</v>
       </c>
       <c r="L15" s="2">
         <v>38</v>
       </c>
-      <c r="M15" s="25">
+      <c r="M15" s="19">
         <v>99</v>
       </c>
       <c r="N15" s="2">
         <v>40</v>
       </c>
-      <c r="O15" s="25">
+      <c r="O15" s="19">
         <v>99</v>
       </c>
       <c r="P15" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="Q15" s="25">
+      <c r="Q15" s="19">
         <v>99</v>
       </c>
       <c r="R15" s="1"/>
@@ -2335,37 +2341,37 @@
       <c r="F16" s="2">
         <v>29</v>
       </c>
-      <c r="G16" s="25">
+      <c r="G16" s="19">
         <v>99</v>
       </c>
       <c r="H16" s="2">
         <v>30</v>
       </c>
-      <c r="I16" s="25">
+      <c r="I16" s="19">
         <v>99</v>
       </c>
       <c r="J16" s="2">
         <v>38</v>
       </c>
-      <c r="K16" s="25">
+      <c r="K16" s="19">
         <v>99</v>
       </c>
       <c r="L16" s="2">
         <v>38</v>
       </c>
-      <c r="M16" s="25">
+      <c r="M16" s="19">
         <v>99</v>
       </c>
       <c r="N16" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="O16" s="25">
+      <c r="O16" s="19">
         <v>99</v>
       </c>
       <c r="P16" s="2">
         <v>40</v>
       </c>
-      <c r="Q16" s="25">
+      <c r="Q16" s="19">
         <v>99</v>
       </c>
       <c r="R16" s="1"/>
@@ -2392,37 +2398,37 @@
       <c r="F17" s="2">
         <v>20</v>
       </c>
-      <c r="G17" s="25">
+      <c r="G17" s="19">
         <v>99</v>
       </c>
       <c r="H17" s="2">
         <v>8</v>
       </c>
-      <c r="I17" s="25">
+      <c r="I17" s="19">
         <v>99</v>
       </c>
       <c r="J17" s="2">
         <v>34</v>
       </c>
-      <c r="K17" s="25">
+      <c r="K17" s="19">
         <v>99</v>
       </c>
       <c r="L17" s="2">
         <v>26</v>
       </c>
-      <c r="M17" s="25">
+      <c r="M17" s="19">
         <v>99</v>
       </c>
       <c r="N17" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="O17" s="25">
+      <c r="O17" s="19">
         <v>99</v>
       </c>
       <c r="P17" s="2">
         <v>40</v>
       </c>
-      <c r="Q17" s="25">
+      <c r="Q17" s="19">
         <v>99</v>
       </c>
       <c r="R17" s="1"/>
@@ -2449,37 +2455,37 @@
       <c r="F18" s="2">
         <v>27</v>
       </c>
-      <c r="G18" s="25">
+      <c r="G18" s="19">
         <v>99</v>
       </c>
       <c r="H18" s="2">
         <v>26</v>
       </c>
-      <c r="I18" s="25">
+      <c r="I18" s="19">
         <v>99</v>
       </c>
       <c r="J18" s="2">
         <v>23</v>
       </c>
-      <c r="K18" s="25">
+      <c r="K18" s="19">
         <v>99</v>
       </c>
       <c r="L18" s="2">
         <v>36</v>
       </c>
-      <c r="M18" s="25">
+      <c r="M18" s="19">
         <v>99</v>
       </c>
       <c r="N18" s="2">
         <v>40</v>
       </c>
-      <c r="O18" s="25">
+      <c r="O18" s="19">
         <v>99</v>
       </c>
       <c r="P18" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="Q18" s="25">
+      <c r="Q18" s="19">
         <v>99</v>
       </c>
       <c r="R18" s="1"/>
@@ -2506,37 +2512,37 @@
       <c r="F19" s="2">
         <v>8</v>
       </c>
-      <c r="G19" s="25">
+      <c r="G19" s="19">
         <v>99</v>
       </c>
       <c r="H19" s="2">
         <v>2</v>
       </c>
-      <c r="I19" s="25">
+      <c r="I19" s="19">
         <v>99</v>
       </c>
       <c r="J19" s="2">
         <v>13</v>
       </c>
-      <c r="K19" s="25">
+      <c r="K19" s="19">
         <v>99</v>
       </c>
       <c r="L19" s="2">
         <v>2</v>
       </c>
-      <c r="M19" s="25">
+      <c r="M19" s="19">
         <v>99</v>
       </c>
       <c r="N19" s="2">
         <v>28</v>
       </c>
-      <c r="O19" s="25">
+      <c r="O19" s="19">
         <v>99</v>
       </c>
       <c r="P19" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="Q19" s="25">
+      <c r="Q19" s="19">
         <v>99</v>
       </c>
       <c r="R19" s="1"/>
@@ -2563,37 +2569,37 @@
       <c r="F20" s="2">
         <v>27</v>
       </c>
-      <c r="G20" s="25">
+      <c r="G20" s="19">
         <v>99</v>
       </c>
       <c r="H20" s="2">
         <v>27</v>
       </c>
-      <c r="I20" s="25">
+      <c r="I20" s="19">
         <v>99</v>
       </c>
       <c r="J20" s="2">
         <v>25</v>
       </c>
-      <c r="K20" s="25">
+      <c r="K20" s="19">
         <v>99</v>
       </c>
       <c r="L20" s="2">
         <v>32</v>
       </c>
-      <c r="M20" s="25">
+      <c r="M20" s="19">
         <v>99</v>
       </c>
       <c r="N20" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="O20" s="25">
+      <c r="O20" s="19">
         <v>99</v>
       </c>
       <c r="P20" s="2">
         <v>39</v>
       </c>
-      <c r="Q20" s="25">
+      <c r="Q20" s="19">
         <v>99</v>
       </c>
       <c r="R20" s="1"/>
@@ -2620,37 +2626,37 @@
       <c r="F21" s="2">
         <v>22</v>
       </c>
-      <c r="G21" s="25">
+      <c r="G21" s="19">
         <v>99</v>
       </c>
       <c r="H21" s="2">
         <v>26</v>
       </c>
-      <c r="I21" s="25">
+      <c r="I21" s="19">
         <v>99</v>
       </c>
       <c r="J21" s="2">
         <v>23</v>
       </c>
-      <c r="K21" s="25">
+      <c r="K21" s="19">
         <v>99</v>
       </c>
       <c r="L21" s="2">
         <v>30</v>
       </c>
-      <c r="M21" s="25">
+      <c r="M21" s="19">
         <v>99</v>
       </c>
       <c r="N21" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="O21" s="25">
+      <c r="O21" s="19">
         <v>99</v>
       </c>
       <c r="P21" s="2">
         <v>40</v>
       </c>
-      <c r="Q21" s="25">
+      <c r="Q21" s="19">
         <v>99</v>
       </c>
       <c r="R21" s="1"/>
@@ -5123,7 +5129,7 @@
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
-  <mergeCells count="8">
+  <mergeCells count="14">
     <mergeCell ref="R9"/>
     <mergeCell ref="A1:H1"/>
     <mergeCell ref="A2:H2"/>
@@ -5132,6 +5138,12 @@
     <mergeCell ref="A5:H5"/>
     <mergeCell ref="A6:H6"/>
     <mergeCell ref="H9:I9"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="F9:G9"/>
+    <mergeCell ref="J9:K9"/>
+    <mergeCell ref="L9:M9"/>
+    <mergeCell ref="N9:O9"/>
+    <mergeCell ref="P9:Q9"/>
   </mergeCells>
   <conditionalFormatting sqref="D11:Q78">
     <cfRule type="cellIs" dxfId="0" priority="1" stopIfTrue="1" operator="lessThan">

</xml_diff>